<commit_message>
updated files after changes
</commit_message>
<xml_diff>
--- a/pythonproject/src/realtime.xlsx
+++ b/pythonproject/src/realtime.xlsx
@@ -440,11 +440,11 @@
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I409" si="1">SWITCH(B2, 
- "D9", CHOOSE(RANDBETWEEN(1,3), 80,85,90),
+ "D9", CHOOSE(RANDBETWEEN(1,3), 10,15,30),
  "D8", CHOOSE(RANDBETWEEN(1,3), 10,15,20),
  "")
 </f>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2">
         <v>0.0</v>
@@ -471,7 +471,7 @@
       </c>
       <c r="I3" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2">
         <v>0.0</v>
@@ -498,7 +498,7 @@
       </c>
       <c r="I4" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2">
         <v>0.0</v>
@@ -525,7 +525,7 @@
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J5" s="2">
         <v>10.0</v>
@@ -552,7 +552,7 @@
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2">
         <v>10.0</v>
@@ -579,7 +579,7 @@
       </c>
       <c r="I7" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J7" s="2">
         <v>10.0</v>
@@ -606,7 +606,7 @@
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J8" s="2">
         <v>10.0</v>
@@ -633,7 +633,7 @@
       </c>
       <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J9" s="2">
         <v>10.0</v>
@@ -660,7 +660,7 @@
       </c>
       <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J10" s="2">
         <v>10.0</v>
@@ -687,7 +687,7 @@
       </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J11" s="2">
         <v>10.0</v>
@@ -714,7 +714,7 @@
       </c>
       <c r="I12" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J12" s="2">
         <v>0.0</v>
@@ -741,7 +741,7 @@
       </c>
       <c r="I13" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J13" s="2">
         <v>0.0</v>
@@ -768,7 +768,7 @@
       </c>
       <c r="I14" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J14" s="2">
         <v>0.0</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="I15" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J15" s="2">
         <v>0.0</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="I16" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J16" s="2">
         <v>0.0</v>
@@ -876,7 +876,7 @@
       </c>
       <c r="I18" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J18" s="2">
         <v>0.0</v>
@@ -903,7 +903,7 @@
       </c>
       <c r="I19" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J19" s="2">
         <v>0.0</v>
@@ -957,7 +957,7 @@
       </c>
       <c r="I21" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J21" s="2">
         <v>0.0</v>
@@ -984,7 +984,7 @@
       </c>
       <c r="I22" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J22" s="2">
         <v>0.0</v>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="I23" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J23" s="2">
         <v>0.0</v>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="I24" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J24" s="2">
         <v>0.0</v>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="I25" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J25" s="2">
         <v>0.0</v>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="I26" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J26" s="2">
         <v>0.0</v>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="I28" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J28" s="2">
         <v>0.0</v>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="I29" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J29" s="2">
         <v>0.0</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="I30" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J30" s="2">
         <v>0.0</v>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="I32" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J32" s="2">
         <v>0.0</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="I33" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J33" s="2">
         <v>0.0</v>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="I34" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J34" s="2">
         <v>0.0</v>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="I35" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J35" s="2">
         <v>0.0</v>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="I36" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J36" s="2">
         <v>0.0</v>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="I38" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J38" s="2">
         <v>0.0</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="I40" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J40" s="2">
         <v>0.0</v>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="I41" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J41" s="2">
         <v>0.0</v>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="I42" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J42" s="2">
         <v>0.0</v>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="I43" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J43" s="2">
         <v>0.0</v>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="I44" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J44" s="2">
         <v>0.0</v>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="I46" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J46" s="2">
         <v>0.0</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="I47" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J47" s="2">
         <v>0.0</v>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="I48" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J48" s="2">
         <v>0.0</v>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="I49" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J49" s="2">
         <v>0.0</v>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="I50" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J50" s="2">
         <v>0.0</v>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="I51" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J51" s="2">
         <v>0.0</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="I52" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J52" s="2">
         <v>0.0</v>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="I53" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J53" s="2">
         <v>0.0</v>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="I54" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J54" s="2">
         <v>0.0</v>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="I55" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J55" s="2">
         <v>0.0</v>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="I56" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J56" s="2">
         <v>0.0</v>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="I57" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J57" s="2">
         <v>0.0</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="I58" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J58" s="2">
         <v>0.0</v>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="I59" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J59" s="2">
         <v>0.0</v>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="I60" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J60" s="2">
         <v>0.0</v>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="I61" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J61" s="2">
         <v>0.0</v>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="I62" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J62" s="2">
         <v>0.0</v>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="I64" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J64" s="2">
         <v>0.0</v>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="I65" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J65" s="2">
         <v>0.0</v>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="I66" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J66" s="2">
         <v>0.0</v>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="I67" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J67" s="2">
         <v>0.0</v>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="I68" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J68" s="2">
         <v>0.0</v>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="I69" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J69" s="2">
         <v>0.0</v>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="I70" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J70" s="2">
         <v>0.0</v>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="I72" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J72" s="2">
         <v>0.0</v>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="I74" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J74" s="2">
         <v>0.0</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="I75" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J75" s="2">
         <v>0.0</v>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="I76" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J76" s="2">
         <v>0.0</v>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="I77" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J77" s="2">
         <v>0.0</v>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="I78" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J78" s="2">
         <v>0.0</v>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="I80" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J80" s="2">
         <v>0.0</v>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="I82" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J82" s="2">
         <v>0.0</v>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="I83" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J83" s="2">
         <v>0.0</v>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="I84" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J84" s="2">
         <v>0.0</v>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="I85" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J85" s="2">
         <v>0.0</v>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="I86" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J86" s="2">
         <v>0.0</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="I87" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J87" s="2">
         <v>0.0</v>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="I88" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J88" s="2">
         <v>0.0</v>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="I90" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J90" s="2">
         <v>0.0</v>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="I91" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J91" s="2">
         <v>20.0</v>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="I93" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J93" s="2">
         <v>0.0</v>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="I98" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J98" s="2">
         <v>0.0</v>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="I99" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J99" s="2">
         <v>0.0</v>
@@ -3090,7 +3090,7 @@
       </c>
       <c r="I100" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J100" s="2">
         <v>0.0</v>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="I101" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J101" s="2">
         <v>0.0</v>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="I103" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J103" s="2">
         <v>0.0</v>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="I104" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J104" s="2">
         <v>10.0</v>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="I105" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J105" s="2">
         <v>0.0</v>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="I107" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J107" s="2">
         <v>10.0</v>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="I108" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J108" s="2">
         <v>0.0</v>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="I109" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J109" s="2">
         <v>10.0</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="I111" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J111" s="2">
         <v>10.0</v>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="I112" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J112" s="2">
         <v>10.0</v>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="I115" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J115" s="2">
         <v>0.0</v>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="I116" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J116" s="2">
         <v>10.0</v>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="I118" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J118" s="2">
         <v>10.0</v>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="I121" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J121" s="2">
         <v>10.0</v>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="I123" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J123" s="2">
         <v>10.0</v>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="I124" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J124" s="2">
         <v>10.0</v>
@@ -3765,7 +3765,7 @@
       </c>
       <c r="I125" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J125" s="2">
         <v>10.0</v>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="I126" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J126" s="2">
         <v>10.0</v>
@@ -3819,7 +3819,7 @@
       </c>
       <c r="I127" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J127" s="2">
         <v>10.0</v>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="I129" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J129" s="2">
         <v>10.0</v>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="I131" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J131" s="2">
         <v>10.0</v>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="I133" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J133" s="2">
         <v>10.0</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="I135" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J135" s="2">
         <v>10.0</v>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="I136" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J136" s="2">
         <v>10.0</v>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="I139" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J139" s="2">
         <v>0.0</v>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="I142" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J142" s="2">
         <v>20.0</v>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="I144" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J144" s="2">
         <v>20.0</v>
@@ -4350,7 +4350,7 @@
       </c>
       <c r="I145" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J145" s="2">
         <v>20.0</v>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="I146" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J146" s="2">
         <v>0.0</v>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="I147" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J147" s="2">
         <v>0.0</v>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="I148" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J148" s="2">
         <v>10.0</v>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="I149" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J149" s="2">
         <v>0.0</v>
@@ -4485,7 +4485,7 @@
       </c>
       <c r="I150" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J150" s="2">
         <v>0.0</v>
@@ -4512,7 +4512,7 @@
       </c>
       <c r="I151" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J151" s="2">
         <v>10.0</v>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="I152" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J152" s="2">
         <v>10.0</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="I153" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J153" s="2">
         <v>0.0</v>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="I154" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J154" s="2">
         <v>10.0</v>
@@ -4620,7 +4620,7 @@
       </c>
       <c r="I155" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J155" s="2">
         <v>0.0</v>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="I157" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J157" s="2">
         <v>0.0</v>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="I158" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J158" s="2">
         <v>0.0</v>
@@ -4728,7 +4728,7 @@
       </c>
       <c r="I159" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J159" s="2">
         <v>0.0</v>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="I160" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J160" s="2">
         <v>0.0</v>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="I161" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J161" s="2">
         <v>0.0</v>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="I162" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J162" s="2">
         <v>0.0</v>
@@ -4836,7 +4836,7 @@
       </c>
       <c r="I163" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J163" s="2">
         <v>0.0</v>
@@ -4863,7 +4863,7 @@
       </c>
       <c r="I164" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J164" s="2">
         <v>0.0</v>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="I165" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J165" s="2">
         <v>0.0</v>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="I166" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J166" s="2">
         <v>0.0</v>
@@ -4944,7 +4944,7 @@
       </c>
       <c r="I167" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J167" s="2">
         <v>0.0</v>
@@ -4971,7 +4971,7 @@
       </c>
       <c r="I168" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J168" s="2">
         <v>0.0</v>
@@ -4998,7 +4998,7 @@
       </c>
       <c r="I169" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J169" s="2">
         <v>0.0</v>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="I170" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J170" s="2">
         <v>0.0</v>
@@ -5052,7 +5052,7 @@
       </c>
       <c r="I171" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J171" s="2">
         <v>0.0</v>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="I172" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J172" s="2">
         <v>0.0</v>
@@ -5106,7 +5106,7 @@
       </c>
       <c r="I173" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J173" s="2">
         <v>0.0</v>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="I174" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J174" s="2">
         <v>0.0</v>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="I175" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J175" s="2">
         <v>0.0</v>
@@ -5214,7 +5214,7 @@
       </c>
       <c r="I177" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J177" s="2">
         <v>20.0</v>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="I178" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J178" s="2">
         <v>0.0</v>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="I179" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J179" s="2">
         <v>10.0</v>
@@ -5295,7 +5295,7 @@
       </c>
       <c r="I180" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J180" s="2">
         <v>30.0</v>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="I181" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J181" s="2">
         <v>10.0</v>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="I182" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J182" s="2">
         <v>0.0</v>
@@ -5376,7 +5376,7 @@
       </c>
       <c r="I183" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J183" s="2">
         <v>0.0</v>
@@ -5403,7 +5403,7 @@
       </c>
       <c r="I184" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J184" s="2">
         <v>0.0</v>
@@ -5430,7 +5430,7 @@
       </c>
       <c r="I185" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J185" s="2">
         <v>0.0</v>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="I186" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J186" s="2">
         <v>0.0</v>
@@ -5484,7 +5484,7 @@
       </c>
       <c r="I187" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J187" s="2">
         <v>0.0</v>
@@ -5511,7 +5511,7 @@
       </c>
       <c r="I188" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J188" s="2">
         <v>0.0</v>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="I189" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J189" s="2">
         <v>0.0</v>
@@ -5565,7 +5565,7 @@
       </c>
       <c r="I190" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J190" s="2">
         <v>0.0</v>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="I191" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J191" s="2">
         <v>0.0</v>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="I192" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J192" s="2">
         <v>0.0</v>
@@ -5673,7 +5673,7 @@
       </c>
       <c r="I194" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J194" s="2">
         <v>0.0</v>
@@ -5700,7 +5700,7 @@
       </c>
       <c r="I195" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J195" s="2">
         <v>0.0</v>
@@ -5727,7 +5727,7 @@
       </c>
       <c r="I196" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J196" s="2">
         <v>0.0</v>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="I197" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J197" s="2">
         <v>0.0</v>
@@ -5781,7 +5781,7 @@
       </c>
       <c r="I198" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J198" s="2">
         <v>0.0</v>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="I199" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J199" s="2">
         <v>0.0</v>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="I200" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J200" s="2">
         <v>0.0</v>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="I201" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J201" s="2">
         <v>0.0</v>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="I202" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J202" s="2">
         <v>0.0</v>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="I203" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J203" s="2">
         <v>0.0</v>
@@ -5943,7 +5943,7 @@
       </c>
       <c r="I204" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J204" s="2">
         <v>0.0</v>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="I205" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J205" s="2">
         <v>0.0</v>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="I206" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J206" s="2">
         <v>0.0</v>
@@ -6024,7 +6024,7 @@
       </c>
       <c r="I207" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J207" s="2">
         <v>0.0</v>
@@ -6051,7 +6051,7 @@
       </c>
       <c r="I208" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J208" s="2">
         <v>0.0</v>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="I209" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J209" s="2">
         <v>0.0</v>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="I210" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J210" s="2">
         <v>0.0</v>
@@ -6132,7 +6132,7 @@
       </c>
       <c r="I211" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J211" s="2">
         <v>0.0</v>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="I212" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J212" s="2">
         <v>0.0</v>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="I213" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J213" s="2">
         <v>0.0</v>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="I214" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J214" s="2">
         <v>0.0</v>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="I215" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J215" s="2">
         <v>0.0</v>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="I216" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J216" s="2">
         <v>0.0</v>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="I217" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J217" s="2">
         <v>0.0</v>
@@ -6321,7 +6321,7 @@
       </c>
       <c r="I218" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J218" s="2">
         <v>0.0</v>
@@ -6348,7 +6348,7 @@
       </c>
       <c r="I219" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J219" s="2">
         <v>0.0</v>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="I220" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J220" s="2">
         <v>0.0</v>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="I221" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J221" s="2">
         <v>0.0</v>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="I222" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J222" s="2">
         <v>20.0</v>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="I223" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J223" s="2">
         <v>10.0</v>
@@ -6483,7 +6483,7 @@
       </c>
       <c r="I224" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J224" s="2">
         <v>10.0</v>
@@ -6510,7 +6510,7 @@
       </c>
       <c r="I225" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J225" s="2">
         <v>10.0</v>
@@ -6537,7 +6537,7 @@
       </c>
       <c r="I226" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J226" s="2">
         <v>0.0</v>
@@ -6564,7 +6564,7 @@
       </c>
       <c r="I227" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J227" s="2">
         <v>0.0</v>
@@ -6591,7 +6591,7 @@
       </c>
       <c r="I228" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J228" s="2">
         <v>20.0</v>
@@ -6618,7 +6618,7 @@
       </c>
       <c r="I229" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J229" s="2">
         <v>10.0</v>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="I230" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J230" s="2">
         <v>0.0</v>
@@ -6672,7 +6672,7 @@
       </c>
       <c r="I231" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J231" s="2">
         <v>10.0</v>
@@ -6699,7 +6699,7 @@
       </c>
       <c r="I232" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J232" s="2">
         <v>0.0</v>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="I233" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J233" s="2">
         <v>0.0</v>
@@ -6753,7 +6753,7 @@
       </c>
       <c r="I234" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J234" s="2">
         <v>10.0</v>
@@ -6780,7 +6780,7 @@
       </c>
       <c r="I235" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J235" s="2">
         <v>0.0</v>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="I236" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J236" s="2">
         <v>10.0</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="I237" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J237" s="2">
         <v>0.0</v>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="I238" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J238" s="2">
         <v>0.0</v>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="I239" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J239" s="2">
         <v>0.0</v>
@@ -6915,7 +6915,7 @@
       </c>
       <c r="I240" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J240" s="2">
         <v>0.0</v>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="I241" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J241" s="2">
         <v>0.0</v>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="I242" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J242" s="2">
         <v>0.0</v>
@@ -6996,7 +6996,7 @@
       </c>
       <c r="I243" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J243" s="2">
         <v>0.0</v>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="I244" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J244" s="2">
         <v>10.0</v>
@@ -7050,7 +7050,7 @@
       </c>
       <c r="I245" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J245" s="2">
         <v>0.0</v>
@@ -7077,7 +7077,7 @@
       </c>
       <c r="I246" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J246" s="2">
         <v>10.0</v>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="I247" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J247" s="2">
         <v>0.0</v>
@@ -7131,7 +7131,7 @@
       </c>
       <c r="I248" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J248" s="2">
         <v>0.0</v>
@@ -7158,7 +7158,7 @@
       </c>
       <c r="I249" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J249" s="2">
         <v>20.0</v>
@@ -7185,7 +7185,7 @@
       </c>
       <c r="I250" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J250" s="2">
         <v>0.0</v>
@@ -7212,7 +7212,7 @@
       </c>
       <c r="I251" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J251" s="2">
         <v>0.0</v>
@@ -7239,7 +7239,7 @@
       </c>
       <c r="I252" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J252" s="2">
         <v>10.0</v>
@@ -7266,7 +7266,7 @@
       </c>
       <c r="I253" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J253" s="2">
         <v>0.0</v>
@@ -7293,7 +7293,7 @@
       </c>
       <c r="I254" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J254" s="2">
         <v>0.0</v>
@@ -7320,7 +7320,7 @@
       </c>
       <c r="I255" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J255" s="2">
         <v>0.0</v>
@@ -7347,7 +7347,7 @@
       </c>
       <c r="I256" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J256" s="2">
         <v>0.0</v>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="I257" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J257" s="2">
         <v>0.0</v>
@@ -7401,7 +7401,7 @@
       </c>
       <c r="I258" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J258" s="2">
         <v>10.0</v>
@@ -7428,7 +7428,7 @@
       </c>
       <c r="I259" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J259" s="2">
         <v>0.0</v>
@@ -7455,7 +7455,7 @@
       </c>
       <c r="I260" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J260" s="2">
         <v>0.0</v>
@@ -7482,7 +7482,7 @@
       </c>
       <c r="I261" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J261" s="2">
         <v>0.0</v>
@@ -7509,7 +7509,7 @@
       </c>
       <c r="I262" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J262" s="2">
         <v>0.0</v>
@@ -7536,7 +7536,7 @@
       </c>
       <c r="I263" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J263" s="2">
         <v>0.0</v>
@@ -7563,7 +7563,7 @@
       </c>
       <c r="I264" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J264" s="2">
         <v>0.0</v>
@@ -7590,7 +7590,7 @@
       </c>
       <c r="I265" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J265" s="2">
         <v>0.0</v>
@@ -7617,7 +7617,7 @@
       </c>
       <c r="I266" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J266" s="2">
         <v>0.0</v>
@@ -7644,7 +7644,7 @@
       </c>
       <c r="I267" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J267" s="2">
         <v>10.0</v>
@@ -7671,7 +7671,7 @@
       </c>
       <c r="I268" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J268" s="2">
         <v>0.0</v>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="I270" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J270" s="2">
         <v>20.0</v>
@@ -7752,7 +7752,7 @@
       </c>
       <c r="I271" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J271" s="2">
         <v>0.0</v>
@@ -7779,7 +7779,7 @@
       </c>
       <c r="I272" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J272" s="2">
         <v>0.0</v>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="I273" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J273" s="2">
         <v>0.0</v>
@@ -7833,7 +7833,7 @@
       </c>
       <c r="I274" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J274" s="2">
         <v>0.0</v>
@@ -7860,7 +7860,7 @@
       </c>
       <c r="I275" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J275" s="2">
         <v>0.0</v>
@@ -7887,7 +7887,7 @@
       </c>
       <c r="I276" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J276" s="2">
         <v>0.0</v>
@@ -7914,7 +7914,7 @@
       </c>
       <c r="I277" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J277" s="2">
         <v>0.0</v>
@@ -7941,7 +7941,7 @@
       </c>
       <c r="I278" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J278" s="2">
         <v>0.0</v>
@@ -7968,7 +7968,7 @@
       </c>
       <c r="I279" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J279" s="2">
         <v>10.0</v>
@@ -7995,7 +7995,7 @@
       </c>
       <c r="I280" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J280" s="2">
         <v>0.0</v>
@@ -8022,7 +8022,7 @@
       </c>
       <c r="I281" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J281" s="2">
         <v>0.0</v>
@@ -8049,7 +8049,7 @@
       </c>
       <c r="I282" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J282" s="2">
         <v>0.0</v>
@@ -8076,7 +8076,7 @@
       </c>
       <c r="I283" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J283" s="2">
         <v>0.0</v>
@@ -8103,7 +8103,7 @@
       </c>
       <c r="I284" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J284" s="2">
         <v>0.0</v>
@@ -8130,7 +8130,7 @@
       </c>
       <c r="I285" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J285" s="2">
         <v>10.0</v>
@@ -8157,7 +8157,7 @@
       </c>
       <c r="I286" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J286" s="2">
         <v>0.0</v>
@@ -8184,7 +8184,7 @@
       </c>
       <c r="I287" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J287" s="2">
         <v>10.0</v>
@@ -8211,7 +8211,7 @@
       </c>
       <c r="I288" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J288" s="2">
         <v>0.0</v>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="I289" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J289" s="2">
         <v>0.0</v>
@@ -8265,7 +8265,7 @@
       </c>
       <c r="I290" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J290" s="2">
         <v>0.0</v>
@@ -8292,7 +8292,7 @@
       </c>
       <c r="I291" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J291" s="2">
         <v>10.0</v>
@@ -8319,7 +8319,7 @@
       </c>
       <c r="I292" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J292" s="2">
         <v>10.0</v>
@@ -8373,7 +8373,7 @@
       </c>
       <c r="I294" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J294" s="2">
         <v>0.0</v>
@@ -8400,7 +8400,7 @@
       </c>
       <c r="I295" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J295" s="2">
         <v>0.0</v>
@@ -8427,7 +8427,7 @@
       </c>
       <c r="I296" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J296" s="2">
         <v>0.0</v>
@@ -8454,7 +8454,7 @@
       </c>
       <c r="I297" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J297" s="2">
         <v>0.0</v>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="I298" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J298" s="2">
         <v>0.0</v>
@@ -8508,7 +8508,7 @@
       </c>
       <c r="I299" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J299" s="2">
         <v>0.0</v>
@@ -8535,7 +8535,7 @@
       </c>
       <c r="I300" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J300" s="2">
         <v>0.0</v>
@@ -8562,7 +8562,7 @@
       </c>
       <c r="I301" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J301" s="2">
         <v>0.0</v>
@@ -8589,7 +8589,7 @@
       </c>
       <c r="I302" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J302" s="2">
         <v>0.0</v>
@@ -8616,7 +8616,7 @@
       </c>
       <c r="I303" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J303" s="2">
         <v>0.0</v>
@@ -8643,7 +8643,7 @@
       </c>
       <c r="I304" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J304" s="2">
         <v>0.0</v>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="I305" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J305" s="2">
         <v>0.0</v>
@@ -8697,7 +8697,7 @@
       </c>
       <c r="I306" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J306" s="2">
         <v>0.0</v>
@@ -8724,7 +8724,7 @@
       </c>
       <c r="I307" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J307" s="2">
         <v>0.0</v>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="I308" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J308" s="2">
         <v>0.0</v>
@@ -8778,7 +8778,7 @@
       </c>
       <c r="I309" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J309" s="2">
         <v>0.0</v>
@@ -8805,7 +8805,7 @@
       </c>
       <c r="I310" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J310" s="2">
         <v>0.0</v>
@@ -8832,7 +8832,7 @@
       </c>
       <c r="I311" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J311" s="2">
         <v>0.0</v>
@@ -8859,7 +8859,7 @@
       </c>
       <c r="I312" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J312" s="2">
         <v>0.0</v>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="I313" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J313" s="2">
         <v>0.0</v>
@@ -8913,7 +8913,7 @@
       </c>
       <c r="I314" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J314" s="2">
         <v>0.0</v>
@@ -8940,7 +8940,7 @@
       </c>
       <c r="I315" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J315" s="2">
         <v>0.0</v>
@@ -8967,7 +8967,7 @@
       </c>
       <c r="I316" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J316" s="2">
         <v>0.0</v>
@@ -8994,7 +8994,7 @@
       </c>
       <c r="I317" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J317" s="2">
         <v>0.0</v>
@@ -9021,7 +9021,7 @@
       </c>
       <c r="I318" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J318" s="2">
         <v>0.0</v>
@@ -9048,7 +9048,7 @@
       </c>
       <c r="I319" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J319" s="2">
         <v>0.0</v>
@@ -9075,7 +9075,7 @@
       </c>
       <c r="I320" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J320" s="2">
         <v>0.0</v>
@@ -9102,7 +9102,7 @@
       </c>
       <c r="I321" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J321" s="2">
         <v>0.0</v>
@@ -9129,7 +9129,7 @@
       </c>
       <c r="I322" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J322" s="2">
         <v>0.0</v>
@@ -9156,7 +9156,7 @@
       </c>
       <c r="I323" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J323" s="2">
         <v>0.0</v>
@@ -9183,7 +9183,7 @@
       </c>
       <c r="I324" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J324" s="2">
         <v>0.0</v>
@@ -9210,7 +9210,7 @@
       </c>
       <c r="I325" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J325" s="2">
         <v>0.0</v>
@@ -9237,7 +9237,7 @@
       </c>
       <c r="I326" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J326" s="2">
         <v>0.0</v>
@@ -9264,7 +9264,7 @@
       </c>
       <c r="I327" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J327" s="2">
         <v>0.0</v>
@@ -9291,7 +9291,7 @@
       </c>
       <c r="I328" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J328" s="2">
         <v>0.0</v>
@@ -9318,7 +9318,7 @@
       </c>
       <c r="I329" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J329" s="2">
         <v>0.0</v>
@@ -9345,7 +9345,7 @@
       </c>
       <c r="I330" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J330" s="2">
         <v>0.0</v>
@@ -9372,7 +9372,7 @@
       </c>
       <c r="I331" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J331" s="2">
         <v>0.0</v>
@@ -9399,7 +9399,7 @@
       </c>
       <c r="I332" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J332" s="2">
         <v>0.0</v>
@@ -9426,7 +9426,7 @@
       </c>
       <c r="I333" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J333" s="2">
         <v>0.0</v>
@@ -9453,7 +9453,7 @@
       </c>
       <c r="I334" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J334" s="2">
         <v>0.0</v>
@@ -9480,7 +9480,7 @@
       </c>
       <c r="I335" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J335" s="2">
         <v>0.0</v>
@@ -9507,7 +9507,7 @@
       </c>
       <c r="I336" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J336" s="2">
         <v>0.0</v>
@@ -9534,7 +9534,7 @@
       </c>
       <c r="I337" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J337" s="2">
         <v>0.0</v>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="I338" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J338" s="2">
         <v>0.0</v>
@@ -9588,7 +9588,7 @@
       </c>
       <c r="I339" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J339" s="2">
         <v>0.0</v>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="I340" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J340" s="2">
         <v>0.0</v>
@@ -9669,7 +9669,7 @@
       </c>
       <c r="I342" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J342" s="2">
         <v>0.0</v>
@@ -9696,7 +9696,7 @@
       </c>
       <c r="I343" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J343" s="2">
         <v>0.0</v>
@@ -9723,7 +9723,7 @@
       </c>
       <c r="I344" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J344" s="2">
         <v>0.0</v>
@@ -9750,7 +9750,7 @@
       </c>
       <c r="I345" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J345" s="2">
         <v>0.0</v>
@@ -9777,7 +9777,7 @@
       </c>
       <c r="I346" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J346" s="2">
         <v>0.0</v>
@@ -9804,7 +9804,7 @@
       </c>
       <c r="I347" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J347" s="2">
         <v>0.0</v>
@@ -9831,7 +9831,7 @@
       </c>
       <c r="I348" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J348" s="2">
         <v>0.0</v>
@@ -9858,7 +9858,7 @@
       </c>
       <c r="I349" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J349" s="2">
         <v>0.0</v>
@@ -9885,7 +9885,7 @@
       </c>
       <c r="I350" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J350" s="2">
         <v>0.0</v>
@@ -9912,7 +9912,7 @@
       </c>
       <c r="I351" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J351" s="2">
         <v>0.0</v>
@@ -9939,7 +9939,7 @@
       </c>
       <c r="I352" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J352" s="2">
         <v>0.0</v>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="I353" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J353" s="2">
         <v>0.0</v>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="I354" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J354" s="2">
         <v>0.0</v>
@@ -10047,7 +10047,7 @@
       </c>
       <c r="I356" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J356" s="2">
         <v>0.0</v>
@@ -10074,7 +10074,7 @@
       </c>
       <c r="I357" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J357" s="2">
         <v>0.0</v>
@@ -10101,7 +10101,7 @@
       </c>
       <c r="I358" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J358" s="2">
         <v>0.0</v>
@@ -10128,7 +10128,7 @@
       </c>
       <c r="I359" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J359" s="2">
         <v>0.0</v>
@@ -10155,7 +10155,7 @@
       </c>
       <c r="I360" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J360" s="2">
         <v>0.0</v>
@@ -10182,7 +10182,7 @@
       </c>
       <c r="I361" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J361" s="2">
         <v>0.0</v>
@@ -10209,7 +10209,7 @@
       </c>
       <c r="I362" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J362" s="2">
         <v>0.0</v>
@@ -10236,7 +10236,7 @@
       </c>
       <c r="I363" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J363" s="2">
         <v>0.0</v>
@@ -10263,7 +10263,7 @@
       </c>
       <c r="I364" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J364" s="2">
         <v>0.0</v>
@@ -10290,7 +10290,7 @@
       </c>
       <c r="I365" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J365" s="2">
         <v>0.0</v>
@@ -10317,7 +10317,7 @@
       </c>
       <c r="I366" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J366" s="2">
         <v>0.0</v>
@@ -10344,7 +10344,7 @@
       </c>
       <c r="I367" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J367" s="2">
         <v>0.0</v>
@@ -10371,7 +10371,7 @@
       </c>
       <c r="I368" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J368" s="2">
         <v>0.0</v>
@@ -10398,7 +10398,7 @@
       </c>
       <c r="I369" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J369" s="2">
         <v>0.0</v>
@@ -10425,7 +10425,7 @@
       </c>
       <c r="I370" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J370" s="2">
         <v>0.0</v>
@@ -10452,7 +10452,7 @@
       </c>
       <c r="I371" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J371" s="2">
         <v>0.0</v>
@@ -10479,7 +10479,7 @@
       </c>
       <c r="I372" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J372" s="2">
         <v>0.0</v>
@@ -10506,7 +10506,7 @@
       </c>
       <c r="I373" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J373" s="2">
         <v>0.0</v>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="I374" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J374" s="2">
         <v>0.0</v>
@@ -10560,7 +10560,7 @@
       </c>
       <c r="I375" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J375" s="2">
         <v>0.0</v>
@@ -10587,7 +10587,7 @@
       </c>
       <c r="I376" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J376" s="2">
         <v>0.0</v>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="I377" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J377" s="2">
         <v>0.0</v>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I378" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J378" s="2">
         <v>0.0</v>
@@ -10668,7 +10668,7 @@
       </c>
       <c r="I379" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J379" s="2">
         <v>0.0</v>
@@ -10695,7 +10695,7 @@
       </c>
       <c r="I380" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J380" s="2">
         <v>0.0</v>
@@ -10722,7 +10722,7 @@
       </c>
       <c r="I381" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J381" s="2">
         <v>0.0</v>
@@ -10749,7 +10749,7 @@
       </c>
       <c r="I382" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J382" s="2">
         <v>0.0</v>
@@ -10776,7 +10776,7 @@
       </c>
       <c r="I383" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J383" s="2">
         <v>0.0</v>
@@ -10803,7 +10803,7 @@
       </c>
       <c r="I384" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J384" s="2">
         <v>0.0</v>
@@ -10830,7 +10830,7 @@
       </c>
       <c r="I385" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J385" s="2">
         <v>0.0</v>
@@ -10857,7 +10857,7 @@
       </c>
       <c r="I386" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J386" s="2">
         <v>0.0</v>
@@ -10884,7 +10884,7 @@
       </c>
       <c r="I387" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J387" s="2">
         <v>0.0</v>
@@ -10911,7 +10911,7 @@
       </c>
       <c r="I388" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J388" s="2">
         <v>0.0</v>
@@ -10938,7 +10938,7 @@
       </c>
       <c r="I389" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J389" s="2">
         <v>0.0</v>
@@ -10965,7 +10965,7 @@
       </c>
       <c r="I390" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J390" s="2">
         <v>0.0</v>
@@ -10992,7 +10992,7 @@
       </c>
       <c r="I391" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J391" s="2">
         <v>0.0</v>
@@ -11019,7 +11019,7 @@
       </c>
       <c r="I392" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J392" s="2">
         <v>0.0</v>
@@ -11046,7 +11046,7 @@
       </c>
       <c r="I393" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J393" s="2">
         <v>0.0</v>
@@ -11073,7 +11073,7 @@
       </c>
       <c r="I394" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J394" s="2">
         <v>0.0</v>
@@ -11100,7 +11100,7 @@
       </c>
       <c r="I395" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J395" s="2">
         <v>0.0</v>
@@ -11127,7 +11127,7 @@
       </c>
       <c r="I396" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J396" s="2">
         <v>0.0</v>
@@ -11154,7 +11154,7 @@
       </c>
       <c r="I397" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J397" s="2">
         <v>0.0</v>
@@ -11181,7 +11181,7 @@
       </c>
       <c r="I398" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J398" s="2">
         <v>0.0</v>
@@ -11208,7 +11208,7 @@
       </c>
       <c r="I399" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J399" s="2">
         <v>0.0</v>
@@ -11235,7 +11235,7 @@
       </c>
       <c r="I400" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="J400" s="2">
         <v>0.0</v>
@@ -11262,7 +11262,7 @@
       </c>
       <c r="I401" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J401" s="2">
         <v>0.0</v>
@@ -11289,7 +11289,7 @@
       </c>
       <c r="I402" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J402" s="2">
         <v>0.0</v>
@@ -11316,7 +11316,7 @@
       </c>
       <c r="I403" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J403" s="2">
         <v>0.0</v>
@@ -11343,7 +11343,7 @@
       </c>
       <c r="I404" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J404" s="2">
         <v>0.0</v>
@@ -11370,7 +11370,7 @@
       </c>
       <c r="I405" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="J405" s="2">
         <v>0.0</v>
@@ -11424,7 +11424,7 @@
       </c>
       <c r="I407" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J407" s="2">
         <v>0.0</v>
@@ -11451,7 +11451,7 @@
       </c>
       <c r="I408" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="J408" s="2">
         <v>0.0</v>
@@ -11478,7 +11478,7 @@
       </c>
       <c r="I409" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J409" s="2">
         <v>0.0</v>

</xml_diff>